<commit_message>
Added a first sentence emphasizer, to put additional emphasis on the first sentence.
</commit_message>
<xml_diff>
--- a/results/Classifier Results.xlsx
+++ b/results/Classifier Results.xlsx
@@ -566,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O45"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="F19" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2531,6 +2531,9 @@
       <c r="O45">
         <v>68.073034536099996</v>
       </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K46" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Further work on SentimentAnalyzer
</commit_message>
<xml_diff>
--- a/results/Classifier Results.xlsx
+++ b/results/Classifier Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="35">
   <si>
     <t>Test Index</t>
   </si>
@@ -204,6 +204,15 @@
   </si>
   <si>
     <t>Combined Corpus</t>
+  </si>
+  <si>
+    <t>Vader</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>First Sentence Emphasizer</t>
   </si>
 </sst>
 </file>
@@ -566,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F19" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD45"/>
+    <sheetView tabSelected="1" topLeftCell="G19" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,17 +586,17 @@
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="37.28515625" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" customWidth="1"/>
+    <col min="5" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="37.28515625" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -595,17 +604,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -622,37 +631,40 @@
         <v>23</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -669,37 +681,40 @@
         <v>24</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6" t="s">
-        <v>13</v>
+      <c r="H6">
+        <v>1</v>
       </c>
       <c r="I6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
         <v>20</v>
       </c>
-      <c r="J6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6">
+      <c r="K6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6">
         <v>65.239294710300001</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>66.126304426100006</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>65.239294710300001</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>58.184670643099999</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -716,37 +731,40 @@
         <v>24</v>
       </c>
       <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>2</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>1</v>
       </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
       <c r="I7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" t="s">
         <v>20</v>
       </c>
-      <c r="J7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L7">
+      <c r="K7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7">
         <v>62.468513853899999</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>65.136322664800005</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>62.468513853899999</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>63.027852020499999</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -763,37 +781,40 @@
         <v>24</v>
       </c>
       <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
         <v>3</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>1</v>
       </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
       <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
         <v>20</v>
       </c>
-      <c r="J8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8">
+      <c r="K8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8">
         <v>62.468513853899999</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>65.483241427799996</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>62.468513853899999</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>63.845343448199998</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -810,37 +831,40 @@
         <v>24</v>
       </c>
       <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
         <v>4</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>1</v>
       </c>
-      <c r="H9" t="s">
-        <v>13</v>
-      </c>
       <c r="I9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" t="s">
         <v>20</v>
       </c>
-      <c r="J9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9">
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9">
         <v>59.697732997499998</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>64.747330187900005</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>59.697732997499998</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>61.8290721531</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -857,37 +881,40 @@
         <v>24</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="H10" t="s">
-        <v>13</v>
+      <c r="H10">
+        <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J10" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10">
+      <c r="K10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10">
         <v>67.758186398000007</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>72.418307373299996</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>67.758186398000007</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>65.565492028099996</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -904,37 +931,40 @@
         <v>24</v>
       </c>
       <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
         <v>2</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>1</v>
       </c>
-      <c r="H11" t="s">
-        <v>13</v>
-      </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J11" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L11">
+      <c r="K11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M11">
         <v>67.506297229200001</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>67.960481582</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>67.506297229200001</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>65.223867239</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
       </c>
@@ -951,37 +981,40 @@
         <v>24</v>
       </c>
       <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
         <v>3</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>1</v>
       </c>
-      <c r="H12" t="s">
-        <v>13</v>
-      </c>
       <c r="I12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J12" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L12">
+      <c r="K12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12">
         <v>69.269521410600007</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>70.074371428800006</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>69.269521410600007</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>68.972128508899999</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
@@ -998,37 +1031,40 @@
         <v>24</v>
       </c>
       <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
         <v>4</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>1</v>
       </c>
-      <c r="H13" t="s">
-        <v>13</v>
-      </c>
       <c r="I13" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J13" t="s">
         <v>18</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L13">
+      <c r="K13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M13">
         <v>65.994962216600001</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>68.195577161700001</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>65.994962216600001</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>66.7062146942</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9</v>
       </c>
@@ -1045,37 +1081,40 @@
         <v>24</v>
       </c>
       <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
         <v>3</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14" t="s">
-        <v>13</v>
+      <c r="H14">
+        <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J14" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L14">
+      <c r="K14" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14">
         <v>72.040302267000001</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>67.8216162688</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>72.040302267000001</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>69.327735838799995</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
@@ -1092,37 +1131,40 @@
         <v>24</v>
       </c>
       <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
         <v>3</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>2</v>
       </c>
-      <c r="H15" t="s">
-        <v>13</v>
-      </c>
       <c r="I15" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J15" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L15">
+      <c r="K15" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15">
         <v>63.979848866499999</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>70.320432086799997</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>63.979848866499999</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>65.571490805099998</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11</v>
       </c>
@@ -1139,37 +1181,40 @@
         <v>24</v>
       </c>
       <c r="F16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <v>3</v>
       </c>
-      <c r="H16" t="s">
-        <v>13</v>
+      <c r="H16">
+        <v>3</v>
       </c>
       <c r="I16" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J16" t="s">
         <v>18</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L16">
+      <c r="K16" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16">
         <v>60.201511334999999</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>71.571376336300006</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>60.201511334999999</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>63.352345351799997</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12</v>
       </c>
@@ -1186,37 +1231,40 @@
         <v>24</v>
       </c>
       <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
         <v>3</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17" t="s">
-        <v>13</v>
+      <c r="H17">
+        <v>0</v>
       </c>
       <c r="I17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" t="s">
         <v>20</v>
       </c>
-      <c r="J17" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L17">
+      <c r="K17" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M17">
         <v>65.491183879100006</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>63.411172825000001</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>65.491183879100006</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>64.418540669999999</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>13</v>
       </c>
@@ -1233,37 +1281,40 @@
         <v>24</v>
       </c>
       <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
         <v>3</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>13</v>
+      <c r="H18">
+        <v>0</v>
       </c>
       <c r="I18" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" t="s">
         <v>21</v>
       </c>
-      <c r="J18" t="s">
-        <v>18</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L18">
+      <c r="K18" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M18">
         <v>65.491183879100006</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>64.040448009299993</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>65.491183879100006</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>64.701304810600007</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>14</v>
       </c>
@@ -1280,37 +1331,40 @@
         <v>24</v>
       </c>
       <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
         <v>3</v>
       </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19" t="s">
-        <v>13</v>
+      <c r="H19">
+        <v>0</v>
       </c>
       <c r="I19" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" t="s">
         <v>21</v>
       </c>
-      <c r="J19" t="s">
-        <v>12</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L19">
+      <c r="K19" t="s">
+        <v>12</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19">
         <v>65.743073047899998</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>63.743648296499998</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>65.743073047899998</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>64.519546417599997</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>15</v>
       </c>
@@ -1327,37 +1381,40 @@
         <v>24</v>
       </c>
       <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
         <v>3</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
-        <v>13</v>
+      <c r="H20">
+        <v>0</v>
       </c>
       <c r="I20" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" t="s">
         <v>20</v>
       </c>
-      <c r="J20" t="s">
-        <v>12</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L20">
+      <c r="K20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M20">
         <v>65.994962216000005</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>63.323466942800003</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>65.994962216600001</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>64.532963552300004</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>16</v>
       </c>
@@ -1374,37 +1431,40 @@
         <v>24</v>
       </c>
       <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
         <v>3</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21" t="s">
-        <v>13</v>
+      <c r="H21">
+        <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J21" t="s">
-        <v>12</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L21">
+        <v>18</v>
+      </c>
+      <c r="K21" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M21">
         <v>72.040302267000001</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>69.049067502400007</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>72.040302267000001</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>69.452911668499993</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>17</v>
       </c>
@@ -1421,37 +1481,40 @@
         <v>24</v>
       </c>
       <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
         <v>2</v>
       </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22" t="s">
-        <v>13</v>
+      <c r="H22">
+        <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J22" t="s">
-        <v>12</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L22">
+        <v>18</v>
+      </c>
+      <c r="K22" t="s">
+        <v>12</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M22">
         <v>71.032745591899996</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>67.106176223600002</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>71.032745591899996</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>66.778704307400005</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>18</v>
       </c>
@@ -1468,37 +1531,40 @@
         <v>24</v>
       </c>
       <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
         <v>1</v>
       </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23" t="s">
-        <v>13</v>
+      <c r="H23">
+        <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J23" t="s">
-        <v>12</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L23">
+        <v>18</v>
+      </c>
+      <c r="K23" t="s">
+        <v>12</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M23">
         <v>69.773299748100001</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>65.334725181099998</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>69.773299748100001</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>64.747930131999993</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>19</v>
       </c>
@@ -1515,37 +1581,40 @@
         <v>24</v>
       </c>
       <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
         <v>3</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>1</v>
       </c>
-      <c r="H24" t="s">
-        <v>13</v>
-      </c>
       <c r="I24" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J24" t="s">
-        <v>12</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L24">
+        <v>18</v>
+      </c>
+      <c r="K24" t="s">
+        <v>12</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M24">
         <v>69.773299748100001</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>70.762648110200004</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>69.773299748100001</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <v>69.092072743800003</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20</v>
       </c>
@@ -1562,37 +1631,40 @@
         <v>24</v>
       </c>
       <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
         <v>3</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>2</v>
       </c>
-      <c r="H25" t="s">
-        <v>13</v>
-      </c>
       <c r="I25" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J25" t="s">
-        <v>12</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L25">
+        <v>18</v>
+      </c>
+      <c r="K25" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M25">
         <v>65.239294710300001</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>71.230790804999998</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>65.239294710300001</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>66.302111348699995</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>21</v>
       </c>
@@ -1609,37 +1681,40 @@
         <v>24</v>
       </c>
       <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
         <v>4</v>
       </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26" t="s">
-        <v>13</v>
+      <c r="H26">
+        <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J26" t="s">
-        <v>12</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L26">
+        <v>18</v>
+      </c>
+      <c r="K26" t="s">
+        <v>12</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M26">
         <v>70.025188916900007</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>66.786399357899995</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <v>70.025188916900007</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <v>68.073034536099996</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>22</v>
       </c>
@@ -1656,37 +1731,40 @@
         <v>24</v>
       </c>
       <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
         <v>3</v>
       </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27" t="s">
-        <v>13</v>
+      <c r="H27">
+        <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J27" t="s">
-        <v>12</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L27">
+        <v>18</v>
+      </c>
+      <c r="K27" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M27">
         <v>61.460957178800001</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>62.951092089399999</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <v>61.460957178800001</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>60.966103408099997</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>23</v>
       </c>
@@ -1703,37 +1781,40 @@
         <v>24</v>
       </c>
       <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
         <v>2</v>
       </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28" t="s">
-        <v>13</v>
+      <c r="H28">
+        <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J28" t="s">
-        <v>12</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L28">
+        <v>18</v>
+      </c>
+      <c r="K28" t="s">
+        <v>12</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M28">
         <v>60.453400503799998</v>
       </c>
-      <c r="M28">
+      <c r="N28">
         <v>63.950014173</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <v>60.453400503799998</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>60.564675988799998</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>24</v>
       </c>
@@ -1750,37 +1831,40 @@
         <v>24</v>
       </c>
       <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
         <v>1</v>
       </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29" t="s">
-        <v>13</v>
+      <c r="H29">
+        <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J29" t="s">
-        <v>12</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L29">
+        <v>18</v>
+      </c>
+      <c r="K29" t="s">
+        <v>12</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M29">
         <v>59.193954659900001</v>
       </c>
-      <c r="M29">
+      <c r="N29">
         <v>65.891164003499995</v>
       </c>
-      <c r="N29">
+      <c r="O29">
         <v>59.193954659900001</v>
       </c>
-      <c r="O29">
+      <c r="P29">
         <v>60.202717700800001</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>25</v>
       </c>
@@ -1797,37 +1881,40 @@
         <v>24</v>
       </c>
       <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
         <v>3</v>
       </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30" t="s">
-        <v>13</v>
+      <c r="H30">
+        <v>0</v>
       </c>
       <c r="I30" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" t="s">
         <v>20</v>
       </c>
-      <c r="J30" t="s">
-        <v>12</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L30">
+      <c r="K30" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M30">
         <v>56.675062972299997</v>
       </c>
-      <c r="M30">
+      <c r="N30">
         <v>62.085875357699997</v>
       </c>
-      <c r="N30">
+      <c r="O30">
         <v>56.675062972299997</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <v>57.689335977399999</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>26</v>
       </c>
@@ -1844,37 +1931,40 @@
         <v>24</v>
       </c>
       <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
         <v>1</v>
       </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31" t="s">
-        <v>13</v>
+      <c r="H31">
+        <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J31" t="s">
-        <v>12</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L31">
+        <v>18</v>
+      </c>
+      <c r="K31" t="s">
+        <v>12</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M31">
         <v>43.073047858899997</v>
       </c>
-      <c r="M31">
+      <c r="N31">
         <v>67.765837884999996</v>
       </c>
-      <c r="N31">
+      <c r="O31">
         <v>43.073047858899997</v>
       </c>
-      <c r="O31">
+      <c r="P31">
         <v>50.7284861487</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>27</v>
       </c>
@@ -1891,37 +1981,40 @@
         <v>24</v>
       </c>
       <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
         <v>2</v>
       </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32" t="s">
-        <v>13</v>
+      <c r="H32">
+        <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J32" t="s">
-        <v>12</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L32">
+        <v>18</v>
+      </c>
+      <c r="K32" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M32">
         <v>52.141057934499997</v>
       </c>
-      <c r="M32">
+      <c r="N32">
         <v>68.359168192599995</v>
       </c>
-      <c r="N32">
+      <c r="O32">
         <v>52.141057934499997</v>
       </c>
-      <c r="O32">
+      <c r="P32">
         <v>57.974126410799997</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>28</v>
       </c>
@@ -1938,37 +2031,40 @@
         <v>24</v>
       </c>
       <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
         <v>3</v>
       </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33" t="s">
-        <v>13</v>
+      <c r="H33">
+        <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J33" t="s">
-        <v>12</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L33">
+        <v>18</v>
+      </c>
+      <c r="K33" t="s">
+        <v>12</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M33">
         <v>53.148614609600003</v>
       </c>
-      <c r="M33">
+      <c r="N33">
         <v>68.412613834499993</v>
       </c>
-      <c r="N33">
+      <c r="O33">
         <v>53.148614609600003</v>
       </c>
-      <c r="O33">
+      <c r="P33">
         <v>58.952701251999997</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>29</v>
       </c>
@@ -1985,37 +2081,40 @@
         <v>24</v>
       </c>
       <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
         <v>4</v>
       </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34" t="s">
-        <v>13</v>
+      <c r="H34">
+        <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J34" t="s">
-        <v>12</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L34">
+        <v>18</v>
+      </c>
+      <c r="K34" t="s">
+        <v>12</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M34">
         <v>53.148614609600003</v>
       </c>
-      <c r="M34">
+      <c r="N34">
         <v>70.440652561199997</v>
       </c>
-      <c r="N34">
+      <c r="O34">
         <v>53.148614609600003</v>
       </c>
-      <c r="O34">
+      <c r="P34">
         <v>59.654738042300004</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>30</v>
       </c>
@@ -2032,37 +2131,40 @@
         <v>24</v>
       </c>
       <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
         <v>4</v>
       </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35" t="s">
-        <v>13</v>
+      <c r="H35">
+        <v>0</v>
       </c>
       <c r="I35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J35" t="s">
         <v>20</v>
       </c>
-      <c r="J35" t="s">
-        <v>12</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L35">
+      <c r="K35" t="s">
+        <v>12</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M35">
         <v>46.095717884099997</v>
       </c>
-      <c r="M35">
+      <c r="N35">
         <v>64.902704813499994</v>
       </c>
-      <c r="N35">
+      <c r="O35">
         <v>46.095717884099997</v>
       </c>
-      <c r="O35">
+      <c r="P35">
         <v>52.989935662900002</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>31</v>
       </c>
@@ -2079,37 +2181,40 @@
         <v>24</v>
       </c>
       <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
         <v>4</v>
       </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36" t="s">
-        <v>13</v>
+      <c r="H36">
+        <v>0</v>
       </c>
       <c r="I36" t="s">
+        <v>13</v>
+      </c>
+      <c r="J36" t="s">
         <v>20</v>
       </c>
-      <c r="J36" t="s">
-        <v>18</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L36">
+      <c r="K36" t="s">
+        <v>18</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M36">
         <v>46.347607052900003</v>
       </c>
-      <c r="M36">
+      <c r="N36">
         <v>65.682826828900005</v>
       </c>
-      <c r="N36">
+      <c r="O36">
         <v>46.347607052900003</v>
       </c>
-      <c r="O36">
+      <c r="P36">
         <v>53.303635988499998</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>32</v>
       </c>
@@ -2126,37 +2231,40 @@
         <v>24</v>
       </c>
       <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
         <v>3</v>
       </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37" t="s">
-        <v>13</v>
+      <c r="H37">
+        <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J37" t="s">
-        <v>12</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L37">
+        <v>18</v>
+      </c>
+      <c r="K37" t="s">
+        <v>12</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M37">
         <v>48.614609571000003</v>
       </c>
-      <c r="M37">
+      <c r="N37">
         <v>67.569426941800003</v>
       </c>
-      <c r="N37">
+      <c r="O37">
         <v>48.614609571800003</v>
       </c>
-      <c r="O37">
+      <c r="P37">
         <v>48.789318432000002</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>33</v>
       </c>
@@ -2173,37 +2281,40 @@
         <v>24</v>
       </c>
       <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
         <v>4</v>
       </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38" t="s">
-        <v>13</v>
+      <c r="H38">
+        <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J38" t="s">
-        <v>12</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L38">
+        <v>18</v>
+      </c>
+      <c r="K38" t="s">
+        <v>12</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M38">
         <v>48.614609571800003</v>
       </c>
-      <c r="M38">
+      <c r="N38">
         <v>71.118104955199996</v>
       </c>
-      <c r="N38">
+      <c r="O38">
         <v>48.614609571800003</v>
       </c>
-      <c r="O38">
+      <c r="P38">
         <v>48.5481997101</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>34</v>
       </c>
@@ -2220,37 +2331,40 @@
         <v>24</v>
       </c>
       <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
         <v>4</v>
       </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39" t="s">
-        <v>13</v>
+      <c r="H39">
+        <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J39" t="s">
-        <v>12</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L39">
+        <v>18</v>
+      </c>
+      <c r="K39" t="s">
+        <v>12</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M39">
         <v>62.720403022699998</v>
       </c>
-      <c r="M39">
+      <c r="N39">
         <v>72.611291950699993</v>
       </c>
-      <c r="N39">
+      <c r="O39">
         <v>62.720403022699998</v>
       </c>
-      <c r="O39">
+      <c r="P39">
         <v>66.8324903484</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>35</v>
       </c>
@@ -2267,37 +2381,40 @@
         <v>24</v>
       </c>
       <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
         <v>3</v>
       </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40" t="s">
-        <v>13</v>
+      <c r="H40">
+        <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J40" t="s">
-        <v>12</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L40">
+        <v>18</v>
+      </c>
+      <c r="K40" t="s">
+        <v>12</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M40">
         <v>61.712846347599999</v>
       </c>
-      <c r="M40">
+      <c r="N40">
         <v>71.735613998600002</v>
       </c>
-      <c r="N40">
+      <c r="O40">
         <v>61.712846347599999</v>
       </c>
-      <c r="O40">
+      <c r="P40">
         <v>65.934067345700001</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>36</v>
       </c>
@@ -2314,37 +2431,40 @@
         <v>24</v>
       </c>
       <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
         <v>5</v>
       </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41" t="s">
-        <v>13</v>
+      <c r="H41">
+        <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J41" t="s">
-        <v>12</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L41">
+        <v>18</v>
+      </c>
+      <c r="K41" t="s">
+        <v>12</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M41">
         <v>60.201511334999999</v>
       </c>
-      <c r="M41">
+      <c r="N41">
         <v>71.437992830100001</v>
       </c>
-      <c r="N41">
+      <c r="O41">
         <v>60.201511334999999</v>
       </c>
-      <c r="O41">
+      <c r="P41">
         <v>64.906025274900003</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>37</v>
       </c>
@@ -2361,37 +2481,40 @@
         <v>24</v>
       </c>
       <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
         <v>3</v>
       </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42" t="s">
-        <v>13</v>
+      <c r="H42">
+        <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J42" t="s">
-        <v>12</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L42">
+        <v>18</v>
+      </c>
+      <c r="K42" t="s">
+        <v>12</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M42">
         <v>65.239294710300001</v>
       </c>
-      <c r="M42">
+      <c r="N42">
         <v>55.755996773200003</v>
       </c>
-      <c r="N42">
+      <c r="O42">
         <v>65.239294710300001</v>
       </c>
-      <c r="O42">
+      <c r="P42">
         <v>59.976411206999998</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>38</v>
       </c>
@@ -2408,37 +2531,40 @@
         <v>24</v>
       </c>
       <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
         <v>2</v>
       </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43" t="s">
-        <v>13</v>
+      <c r="H43">
+        <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J43" t="s">
-        <v>12</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L43">
+        <v>18</v>
+      </c>
+      <c r="K43" t="s">
+        <v>12</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M43">
         <v>65.743073047899998</v>
       </c>
-      <c r="M43">
+      <c r="N43">
         <v>59.525861252600002</v>
       </c>
-      <c r="N43">
+      <c r="O43">
         <v>65.743073047899998</v>
       </c>
-      <c r="O43">
+      <c r="P43">
         <v>59.187192032200002</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>39</v>
       </c>
@@ -2455,37 +2581,40 @@
         <v>24</v>
       </c>
       <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
         <v>1</v>
       </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-      <c r="H44" t="s">
-        <v>13</v>
+      <c r="H44">
+        <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J44" t="s">
-        <v>12</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L44">
+        <v>18</v>
+      </c>
+      <c r="K44" t="s">
+        <v>12</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M44">
         <v>66.246851385400007</v>
       </c>
-      <c r="M44">
+      <c r="N44">
         <v>50.784380624999997</v>
       </c>
-      <c r="N44">
+      <c r="O44">
         <v>66.246851385400007</v>
       </c>
-      <c r="O44">
+      <c r="P44">
         <v>57.488929750399997</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>40</v>
       </c>
@@ -2502,38 +2631,188 @@
         <v>24</v>
       </c>
       <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
         <v>4</v>
       </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45" t="s">
-        <v>13</v>
+      <c r="H45">
+        <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="J45" t="s">
-        <v>12</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L45">
+        <v>18</v>
+      </c>
+      <c r="K45" t="s">
+        <v>12</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M45">
         <v>70.025188916900007</v>
       </c>
-      <c r="M45">
+      <c r="N45">
         <v>66.786399357899995</v>
       </c>
-      <c r="N45">
+      <c r="O45">
         <v>70.025188916900007</v>
       </c>
-      <c r="O45">
+      <c r="P45">
         <v>68.073034536099996</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="K46" s="1"/>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>41</v>
+      </c>
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46" t="s">
+        <v>13</v>
+      </c>
+      <c r="J46" t="s">
+        <v>18</v>
+      </c>
+      <c r="K46" t="s">
+        <v>12</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M46">
+        <v>46.347607052900003</v>
+      </c>
+      <c r="N46">
+        <v>79.006972176399998</v>
+      </c>
+      <c r="O46">
+        <v>46.347607052900003</v>
+      </c>
+      <c r="P46">
+        <v>52.071164363400001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>42</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" t="s">
+        <v>33</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>2</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47" t="s">
+        <v>13</v>
+      </c>
+      <c r="J47" t="s">
+        <v>18</v>
+      </c>
+      <c r="K47" t="s">
+        <v>12</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M47">
+        <v>44.080604534000003</v>
+      </c>
+      <c r="N47">
+        <v>74.471145158499993</v>
+      </c>
+      <c r="O47">
+        <v>44.080604534000003</v>
+      </c>
+      <c r="P47">
+        <v>50.350292062500003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>43</v>
+      </c>
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48" t="s">
+        <v>13</v>
+      </c>
+      <c r="J48" t="s">
+        <v>18</v>
+      </c>
+      <c r="K48" t="s">
+        <v>12</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M48">
+        <v>13.6020151134</v>
+      </c>
+      <c r="N48">
+        <v>89.240542161400001</v>
+      </c>
+      <c r="O48">
+        <v>13.6020151134</v>
+      </c>
+      <c r="P48">
+        <v>11.179136613900001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>